<commit_message>
Update of CO - NO2 Values for calibration.xlsx
</commit_message>
<xml_diff>
--- a/NO2-CO-Measurement/CO - NO2 Values for calibration.xlsx
+++ b/NO2-CO-Measurement/CO - NO2 Values for calibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msanti/Documents/Arduino/CJMCU-4514-Calibration Example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msanti/Documents/CSC 1- Barcelona/CJMCU-4514/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D511753-0D83-FF46-8A10-B67A070438A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E962EE6A-1E10-6949-BF49-8DEF856B1FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" xr2:uid="{2AAEF7E2-FAB7-FD4A-BAE6-F65137EF0357}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{2AAEF7E2-FAB7-FD4A-BAE6-F65137EF0357}"/>
   </bookViews>
   <sheets>
     <sheet name="NO2" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,50 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={77757DFB-70AD-7C46-8B07-8A0C1B7C2505}</author>
+  </authors>
+  <commentList>
+    <comment ref="E24" authorId="0" shapeId="0" xr:uid="{77757DFB-70AD-7C46-8B07-8A0C1B7C2505}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Traducción de Alemán a Español:
+Para determinar las fórmulas de conversión de la resistencia del sensor Rs a ppm (partes por millón), algunos puntos de datos deben extraerse del diagrama respectivo del sensor del data sheet y transferirse a Excel, por ejemplo. Dado que es (principalmente) una escala logarítmica en los ejes x e y, estos valores deben convertirse con = log (Rs / R0) o = log (ppm).
+El resultado de estas nuevas columnas de registro se muestra en un diagrama x / y y se inserta una línea de tendencia lineal a través del menú de propiedades de la serie de datos. Para obtener la fórmula de la línea de tendencia, debe mostrarse bajo las propiedades de la línea de tendencia. La fórmula de la línea de tendencia se utiliza para convertir Rs / R0 en un valor de ppm.
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BA5F9A3E-02AF-724A-95A3-B07F9C984745}</author>
+  </authors>
+  <commentList>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{BA5F9A3E-02AF-724A-95A3-B07F9C984745}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Traducción de Alemán a Español:
+Para determinar las fórmulas de conversión de la resistencia del sensor Rs a ppm (partes por millón), algunos puntos de datos deben extraerse del diagrama respectivo del sensor del data sheet y transferirse a Excel, por ejemplo. Dado que es (principalmente) una escala logarítmica en los ejes x e y, estos valores deben convertirse con = log (Rs / R0) o = log (ppm).
+El resultado de estas nuevas columnas de registro se muestra en un diagrama x / y y se inserta una línea de tendencia lineal a través del menú de propiedades de la serie de datos. Para obtener la fórmula de la línea de tendencia, debe mostrarse bajo las propiedades de la línea de tendencia. La fórmula de la línea de tendencia se utiliza para convertir Rs / R0 en un valor de ppm.
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>NO2</t>
   </si>
@@ -56,21 +98,6 @@
   </si>
   <si>
     <t>0,05 – 10 ppm</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">From Datasheet: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://www.sgxsensortech.com/content/uploads/2014/08/0278_Datasheet-MiCS-4514.pdf</t>
-    </r>
   </si>
   <si>
     <r>
@@ -112,12 +139,6 @@
     <t>1 - 1000 ppm</t>
   </si>
   <si>
-    <t>R0 0,8k-20kΩ(to be measured)</t>
-  </si>
-  <si>
-    <t>R0 100 - 1500kΩ(to be measured)</t>
-  </si>
-  <si>
     <t>RLoad 22kΩ</t>
   </si>
   <si>
@@ -130,17 +151,35 @@
     <t>ppm = pow(10, 0.9682*log(Rs/R0) - 0.8108)</t>
   </si>
   <si>
-    <t>Saco</t>
+    <t xml:space="preserve">R0 = RS / POW(10, ( (log10(NO2ppm) + 0,8108 ) / 0,9682 )) </t>
   </si>
   <si>
-    <t>1) Valor medido de NO2 = 0.59ppm;  valor medido de Rs = 3563.69</t>
+    <t>R0 = RS / POW(10, ( (log10(COppm) - 0,6201) / -1,1859 ) )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://myscope.net/auswertung-der-airpi-gas-sensoren/</t>
+  </si>
+  <si>
+    <t>https://www.sgxsensortech.com/content/uploads/2014/08/0278_Datasheet-MiCS-4514.pdf</t>
+  </si>
+  <si>
+    <t>Datasheet Values</t>
+  </si>
+  <si>
+    <t>Instructions in:</t>
+  </si>
+  <si>
+    <t>R0 100 - 1500kΩ(to be measured)/ We put 200 Ω int he code</t>
+  </si>
+  <si>
+    <t>R0 0,8k-20kΩ(to be measured)/ We put 900 Ω in the code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +232,20 @@
       <color rgb="FF2B2B2B"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -214,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -237,22 +290,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,12 +326,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,8 +341,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4947,6 +5018,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="MARISOL SANTILLAN" id="{E19F4922-2E65-C049-8265-600CACA0C280}" userId="S::msanti@ar.ibm.com::5267b941-c424-427e-999c-d2d35535d93c" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5242,11 +5319,35 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E24" dT="2020-12-16T03:08:06.58" personId="{E19F4922-2E65-C049-8265-600CACA0C280}" id="{77757DFB-70AD-7C46-8B07-8A0C1B7C2505}">
+    <text xml:space="preserve">Traducción de Alemán a Español:
+Para determinar las fórmulas de conversión de la resistencia del sensor Rs a ppm (partes por millón), algunos puntos de datos deben extraerse del diagrama respectivo del sensor del data sheet y transferirse a Excel, por ejemplo. Dado que es (principalmente) una escala logarítmica en los ejes x e y, estos valores deben convertirse con = log (Rs / R0) o = log (ppm).
+El resultado de estas nuevas columnas de registro se muestra en un diagrama x / y y se inserta una línea de tendencia lineal a través del menú de propiedades de la serie de datos. Para obtener la fórmula de la línea de tendencia, debe mostrarse bajo las propiedades de la línea de tendencia. La fórmula de la línea de tendencia se utiliza para convertir Rs / R0 en un valor de ppm.
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E18" dT="2020-12-16T03:09:31.14" personId="{E19F4922-2E65-C049-8265-600CACA0C280}" id="{BA5F9A3E-02AF-724A-95A3-B07F9C984745}">
+    <text xml:space="preserve">Traducción de Alemán a Español:
+Para determinar las fórmulas de conversión de la resistencia del sensor Rs a ppm (partes por millón), algunos puntos de datos deben extraerse del diagrama respectivo del sensor del data sheet y transferirse a Excel, por ejemplo. Dado que es (principalmente) una escala logarítmica en los ejes x e y, estos valores deben convertirse con = log (Rs / R0) o = log (ppm).
+El resultado de estas nuevas columnas de registro se muestra en un diagrama x / y y se inserta una línea de tendencia lineal a través del menú de propiedades de la serie de datos. Para obtener la fórmula de la línea de tendencia, debe mostrarse bajo las propiedades de la línea de tendencia. La fórmula de la línea de tendencia se utiliza para convertir Rs / R0 en un valor de ppm.
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AA835B-B3E0-814C-8E29-57C2843FA815}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AA835B-B3E0-814C-8E29-57C2843FA815}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0"/>
+    <sheetView zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5267,10 +5368,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5280,21 +5378,30 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
+    <row r="7" spans="1:5" ht="31" customHeight="1">
+      <c r="A7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" ht="18">
       <c r="A8" s="3" t="s">
@@ -5310,7 +5417,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18">
@@ -5494,77 +5601,76 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="18">
-      <c r="A18" s="12">
-        <v>5.66</v>
-      </c>
-      <c r="C18" s="13">
-        <f t="shared" si="0"/>
-        <v>0.75281643118827146</v>
-      </c>
-      <c r="E18" s="11">
-        <f t="shared" si="2"/>
-        <v>0.82808871968667452</v>
-      </c>
+      <c r="A18" s="15"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="28"/>
     </row>
     <row r="19" spans="1:5" ht="18">
-      <c r="A19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
+      <c r="A19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="28"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="E21" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" ht="18">
-      <c r="A22" s="1">
-        <v>3.96</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.59</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" ref="C22" si="3">LOG10((A22))</f>
-        <v>0.5976951859255123</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" ref="D22" si="4">LOG10((B22))</f>
-        <v>-0.22914798835785583</v>
-      </c>
-      <c r="E22" s="11">
-        <f t="shared" ref="E22" si="5">POWER(10,0.9682*C22-0.8108)</f>
-        <v>0.58598767143301267</v>
-      </c>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="18">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B24" r:id="rId1" xr:uid="{BFC47E3D-2DF2-2940-BA90-BE04F7338597}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{56605B29-55A0-7D41-AE4B-71542072BC58}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCAFCA-3CE9-DC49-A954-9ED3A38F03D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCAFCA-3CE9-DC49-A954-9ED3A38F03D2}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -5574,44 +5680,47 @@
     <col min="5" max="5" width="41.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" ht="48" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="16"/>
+    <row r="1" spans="1:5" s="13" customFormat="1" ht="48" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
+    <row r="7" spans="1:5" ht="34">
+      <c r="A7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18">
@@ -5628,7 +5737,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18">
@@ -5647,8 +5756,8 @@
         <v>-9.6910013008056392E-2</v>
       </c>
       <c r="E9" s="11">
-        <f>-1.1859*C9 + 0.6201</f>
-        <v>-9.3882943715830613E-2</v>
+        <f>POWER(10, -1.1859*C9 + 0.6201)</f>
+        <v>0.80559554576235659</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18">
@@ -5659,7 +5768,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" ref="C10:D16" si="0">LOG10((A10))</f>
+        <f t="shared" ref="C10:D14" si="0">LOG10((A10))</f>
         <v>0</v>
       </c>
       <c r="D10" s="2">
@@ -5667,8 +5776,8 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="E10" s="11">
-        <f t="shared" ref="E10:E14" si="1">-1.1859*C10 + 0.6201</f>
-        <v>0.62009999999999998</v>
+        <f t="shared" ref="E10:E14" si="1">POWER(10, -1.1859*C10 + 0.6201)</f>
+        <v>4.1696538224498916</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18">
@@ -5688,7 +5797,7 @@
       </c>
       <c r="E11" s="11">
         <f t="shared" si="1"/>
-        <v>0.97709147185791534</v>
+        <v>9.4861824188265</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18">
@@ -5708,7 +5817,7 @@
       </c>
       <c r="E12" s="11">
         <f t="shared" si="1"/>
-        <v>1.806</v>
+        <v>63.973483548264831</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18">
@@ -5728,7 +5837,7 @@
       </c>
       <c r="E13" s="11">
         <f t="shared" si="1"/>
-        <v>2.1629914718579153</v>
+        <v>145.54305003432438</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18">
@@ -5748,31 +5857,41 @@
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
-        <v>2.9918999999999998</v>
+        <v>981.52191322575754</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18">
-      <c r="B16" s="17"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="15"/>
+      <c r="D16" s="18"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+    <row r="18" spans="1:5" ht="18">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="D22" s="18"/>
+    <row r="22" spans="1:5">
+      <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:4">
-      <c r="D23" s="18"/>
+    <row r="23" spans="1:5">
+      <c r="D23" s="16"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{DA004C2C-4924-1547-AFDA-A0ABD77A0612}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{888EDB3D-C389-F745-9771-11BFCC66142C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>